<commit_message>
Actualizado del 610 al 614
</commit_message>
<xml_diff>
--- a/normativa/Anexos/L05T02C03/L05T02C03A04.9.xlsx
+++ b/normativa/Anexos/L05T02C03/L05T02C03A04.9.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -10,14 +10,14 @@
     <sheet name="HOJA 2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'HOJA 2'!$A$1:$K$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'HOJA 2'!$A$1:$K$66</definedName>
   </definedNames>
   <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>Contador General</t>
   </si>
@@ -101,21 +101,9 @@
     <t>HIPOTECARIO DE VIVIENDA</t>
   </si>
   <si>
-    <t>i) Adquisición de terreno para la construcción de vivienda</t>
-  </si>
-  <si>
-    <t>ii) Construcción de vivienda individual</t>
-  </si>
-  <si>
     <t>iii) Compra de vivienda individual o en propiedad horizontal</t>
   </si>
   <si>
-    <t xml:space="preserve">iv) Refacción, remodelación, ampliación, mejoramiento de </t>
-  </si>
-  <si>
-    <t>vivienda individual o en propiedad horizontal</t>
-  </si>
-  <si>
     <t>CONSUMO</t>
   </si>
   <si>
@@ -147,6 +135,66 @@
   </si>
   <si>
     <t>LIBRO 5°, TÍTULO II, CAPÍTULO III</t>
+  </si>
+  <si>
+    <t>CRÉDITO DE VIVIENDA SIN GARANTÍA HIPOTECARIA</t>
+  </si>
+  <si>
+    <t>i) Contrucción de vivienda individual o en propiedad horizontal</t>
+  </si>
+  <si>
+    <t>ii) Refacción, remodelación, ampliación, mejoramiento de vivienda individual o en propiedad horizontal</t>
+  </si>
+  <si>
+    <t>iii) Anticrético de vivienda individual o en propiedad horizontal</t>
+  </si>
+  <si>
+    <t>CRÉDITO DE VIVIENDA SIN GARANTÍA HIPOTECARIA DEBIDAMENTE GARANTIZADO</t>
+  </si>
+  <si>
+    <t>HIPOTECARIO DE VIVIENDA DE INTERÉS SOCIAL</t>
+  </si>
+  <si>
+    <t>ii) Compra de vivienda individual o en propiedad horizontal</t>
+  </si>
+  <si>
+    <t>iii) Construcción de vivienda individual o en propiedad horizontal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRÉDITO DE VIVIENDA DE INTERÉS SOCIAL SIN GARANTÍA HIPOTECARIA </t>
+  </si>
+  <si>
+    <t>i) Construcción de vivienda individual o en propiedad horizontal</t>
+  </si>
+  <si>
+    <t>iv) Créditos otorgados a personas asalariadas que por cuenta de su empleador perciben el pago de su salario en la misma entidad</t>
+  </si>
+  <si>
+    <t>iv) Refacción, remodelación, ampliación, mejoramiento de vivienda
+     individual o en propiedad horizontal</t>
+  </si>
+  <si>
+    <t>ii) Refacción, remodelación, ampliación, mejoramiento de vivienda 
+    individual o en propiedad horizontal</t>
+  </si>
+  <si>
+    <t>ii) Refacción, remodelación, ampliación, mejoramiento de vivienda  
+    individual o en propiedad horizontal</t>
+  </si>
+  <si>
+    <t>i) Adquisición de terreno con fines de construcción de vivienda  
+   individual o en propiedad horizontal</t>
+  </si>
+  <si>
+    <t>iv) Refacción, remodelación, ampliación, mejoramiento de vivienda  
+     individual o en propiedad horizontal</t>
+  </si>
+  <si>
+    <t>i) Adquisición de terreno para la construcción de vivienda individual
+   o en propiedad horizontal</t>
+  </si>
+  <si>
+    <t>ii) Construcción de vivienda individual o en propiedad horizontal</t>
   </si>
 </sst>
 </file>
@@ -260,7 +308,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -364,13 +412,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="39" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="39" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -408,9 +478,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -421,15 +488,47 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -459,6 +558,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -507,7 +609,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -542,7 +644,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -751,15 +853,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE47"/>
+  <dimension ref="A1:AE67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="53.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
@@ -803,19 +905,19 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:31" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
+      <c r="A2" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -1050,29 +1152,29 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:31" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="31" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="31" t="s">
+      <c r="E10" s="41"/>
+      <c r="F10" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="32"/>
-      <c r="H10" s="31" t="s">
+      <c r="G10" s="41"/>
+      <c r="H10" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="32"/>
-      <c r="J10" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="32"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="41"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1091,35 +1193,35 @@
       <c r="AA10" s="2"/>
     </row>
     <row r="11" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
-      <c r="B11" s="29" t="s">
+      <c r="A11" s="45"/>
+      <c r="B11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="29" t="s">
+      <c r="C11" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="29" t="s">
+      <c r="E11" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="29" t="s">
+      <c r="G11" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="30" t="s">
+      <c r="J11" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="26" t="s">
         <v>18</v>
       </c>
       <c r="L11" s="2"/>
@@ -1139,7 +1241,7 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" spans="1:31" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
@@ -1168,9 +1270,9 @@
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
     </row>
-    <row r="13" spans="1:31" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>38</v>
+    <row r="13" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="B13" s="17"/>
       <c r="C13" s="18"/>
@@ -1199,8 +1301,8 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" spans="1:31" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+    <row r="14" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="17"/>
@@ -1230,8 +1332,8 @@
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
     </row>
-    <row r="15" spans="1:31" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+    <row r="15" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="17"/>
@@ -1261,8 +1363,8 @@
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
     </row>
-    <row r="16" spans="1:31" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+    <row r="16" spans="1:31" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
       <c r="D16" s="17"/>
@@ -1290,8 +1392,8 @@
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
     </row>
-    <row r="17" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+    <row r="17" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="17"/>
@@ -1321,8 +1423,8 @@
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
     </row>
-    <row r="18" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+    <row r="18" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="17"/>
@@ -1352,8 +1454,8 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
     </row>
-    <row r="19" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+    <row r="19" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="17"/>
@@ -1383,8 +1485,8 @@
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
     </row>
-    <row r="20" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
+    <row r="20" spans="1:27" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
       <c r="B20" s="17"/>
       <c r="C20" s="18"/>
       <c r="D20" s="17"/>
@@ -1412,8 +1514,8 @@
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
     </row>
-    <row r="21" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+    <row r="21" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="17"/>
@@ -1443,8 +1545,8 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+    <row r="22" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="17"/>
@@ -1474,8 +1576,8 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
     </row>
-    <row r="23" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+    <row r="23" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="17"/>
@@ -1505,8 +1607,8 @@
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
     </row>
-    <row r="24" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
+    <row r="24" spans="1:27" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
       <c r="B24" s="17"/>
       <c r="C24" s="18"/>
       <c r="D24" s="17"/>
@@ -1534,8 +1636,8 @@
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
     </row>
-    <row r="25" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+    <row r="25" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="17"/>
@@ -1565,9 +1667,9 @@
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
     </row>
-    <row r="26" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
-        <v>24</v>
+    <row r="26" spans="1:27" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="29" t="s">
+        <v>52</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="18"/>
@@ -1596,9 +1698,9 @@
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
     </row>
-    <row r="27" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>25</v>
+    <row r="27" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>53</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="18"/>
@@ -1627,9 +1729,9 @@
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
     </row>
-    <row r="28" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>26</v>
+    <row r="28" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
+        <v>24</v>
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="18"/>
@@ -1658,9 +1760,9 @@
       <c r="Z28" s="2"/>
       <c r="AA28" s="2"/>
     </row>
-    <row r="29" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
-        <v>27</v>
+    <row r="29" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>47</v>
       </c>
       <c r="B29" s="17"/>
       <c r="C29" s="18"/>
@@ -1689,10 +1791,8 @@
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
     </row>
-    <row r="30" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
-        <v>28</v>
-      </c>
+    <row r="30" spans="1:27" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="27"/>
       <c r="B30" s="17"/>
       <c r="C30" s="18"/>
       <c r="D30" s="17"/>
@@ -1720,8 +1820,10 @@
       <c r="Z30" s="2"/>
       <c r="AA30" s="2"/>
     </row>
-    <row r="31" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
+    <row r="31" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="B31" s="17"/>
       <c r="C31" s="18"/>
       <c r="D31" s="17"/>
@@ -1749,9 +1851,9 @@
       <c r="Z31" s="2"/>
       <c r="AA31" s="2"/>
     </row>
-    <row r="32" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
-        <v>29</v>
+    <row r="32" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="29" t="s">
+        <v>37</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="18"/>
@@ -1780,9 +1882,9 @@
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
     </row>
-    <row r="33" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
-        <v>30</v>
+    <row r="33" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="29" t="s">
+        <v>48</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="18"/>
@@ -1811,9 +1913,9 @@
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
     </row>
-    <row r="34" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
-        <v>31</v>
+    <row r="34" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="29" t="s">
+        <v>39</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="18"/>
@@ -1842,10 +1944,8 @@
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
     </row>
-    <row r="35" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
-        <v>32</v>
-      </c>
+    <row r="35" spans="1:27" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
       <c r="B35" s="17"/>
       <c r="C35" s="18"/>
       <c r="D35" s="17"/>
@@ -1873,18 +1973,20 @@
       <c r="Z35" s="2"/>
       <c r="AA35" s="2"/>
     </row>
-    <row r="36" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="21"/>
+    <row r="36" spans="1:27" ht="24" x14ac:dyDescent="0.25">
+      <c r="A36" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="18"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -1902,20 +2004,20 @@
       <c r="Z36" s="2"/>
       <c r="AA36" s="2"/>
     </row>
-    <row r="37" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="24"/>
+    <row r="37" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="17"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="18"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -1933,20 +2035,20 @@
       <c r="Z37" s="2"/>
       <c r="AA37" s="2"/>
     </row>
-    <row r="38" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="26"/>
-      <c r="K38" s="26"/>
+    <row r="38" spans="1:27" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="18"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -1964,20 +2066,18 @@
       <c r="Z38" s="2"/>
       <c r="AA38" s="2"/>
     </row>
-    <row r="39" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="26"/>
-      <c r="K39" s="26"/>
+    <row r="39" spans="1:27" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="29"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="18"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -1995,111 +2095,725 @@
       <c r="Z39" s="2"/>
       <c r="AA39" s="2"/>
     </row>
-    <row r="40" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-    </row>
-    <row r="41" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-    </row>
-    <row r="43" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+    <row r="40" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="17"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2"/>
+      <c r="Y40" s="2"/>
+      <c r="Z40" s="2"/>
+      <c r="AA40" s="2"/>
+    </row>
+    <row r="41" spans="1:27" ht="24" x14ac:dyDescent="0.25">
+      <c r="A41" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="17"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2"/>
+      <c r="Y41" s="2"/>
+      <c r="Z41" s="2"/>
+      <c r="AA41" s="2"/>
+    </row>
+    <row r="42" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="17"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2"/>
+      <c r="Y42" s="2"/>
+      <c r="Z42" s="2"/>
+      <c r="AA42" s="2"/>
+    </row>
+    <row r="43" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="17"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2"/>
+      <c r="Y43" s="2"/>
+      <c r="Z43" s="2"/>
+      <c r="AA43" s="2"/>
+    </row>
+    <row r="44" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+      <c r="X44" s="2"/>
+      <c r="Y44" s="2"/>
+      <c r="Z44" s="2"/>
+      <c r="AA44" s="2"/>
+    </row>
+    <row r="45" spans="1:27" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="32"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
+      <c r="U45" s="2"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
+      <c r="X45" s="2"/>
+      <c r="Y45" s="2"/>
+      <c r="Z45" s="2"/>
+      <c r="AA45" s="2"/>
+    </row>
+    <row r="46" spans="1:27" ht="24" x14ac:dyDescent="0.25">
+      <c r="A46" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="36"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="36"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+      <c r="S46" s="2"/>
+      <c r="T46" s="2"/>
+      <c r="U46" s="2"/>
+      <c r="V46" s="2"/>
+      <c r="W46" s="2"/>
+      <c r="X46" s="2"/>
+      <c r="Y46" s="2"/>
+      <c r="Z46" s="2"/>
+      <c r="AA46" s="2"/>
+    </row>
+    <row r="47" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="17"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
+      <c r="V47" s="2"/>
+      <c r="W47" s="2"/>
+      <c r="X47" s="2"/>
+      <c r="Y47" s="2"/>
+      <c r="Z47" s="2"/>
+      <c r="AA47" s="2"/>
+    </row>
+    <row r="48" spans="1:27" ht="24" x14ac:dyDescent="0.25">
+      <c r="A48" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="17"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+      <c r="S48" s="2"/>
+      <c r="T48" s="2"/>
+      <c r="U48" s="2"/>
+      <c r="V48" s="2"/>
+      <c r="W48" s="2"/>
+      <c r="X48" s="2"/>
+      <c r="Y48" s="2"/>
+      <c r="Z48" s="2"/>
+      <c r="AA48" s="2"/>
+    </row>
+    <row r="49" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="17"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+      <c r="U49" s="2"/>
+      <c r="V49" s="2"/>
+      <c r="W49" s="2"/>
+      <c r="X49" s="2"/>
+      <c r="Y49" s="2"/>
+      <c r="Z49" s="2"/>
+      <c r="AA49" s="2"/>
+    </row>
+    <row r="50" spans="1:27" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="27"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+      <c r="U50" s="2"/>
+      <c r="V50" s="2"/>
+      <c r="W50" s="2"/>
+      <c r="X50" s="2"/>
+      <c r="Y50" s="2"/>
+      <c r="Z50" s="2"/>
+      <c r="AA50" s="2"/>
+    </row>
+    <row r="51" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="17"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="17"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
+      <c r="S51" s="2"/>
+      <c r="T51" s="2"/>
+      <c r="U51" s="2"/>
+      <c r="V51" s="2"/>
+      <c r="W51" s="2"/>
+      <c r="X51" s="2"/>
+      <c r="Y51" s="2"/>
+      <c r="Z51" s="2"/>
+      <c r="AA51" s="2"/>
+    </row>
+    <row r="52" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="17"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="17"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+      <c r="S52" s="2"/>
+      <c r="T52" s="2"/>
+      <c r="U52" s="2"/>
+      <c r="V52" s="2"/>
+      <c r="W52" s="2"/>
+      <c r="X52" s="2"/>
+      <c r="Y52" s="2"/>
+      <c r="Z52" s="2"/>
+      <c r="AA52" s="2"/>
+    </row>
+    <row r="53" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" s="17"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="2"/>
+      <c r="S53" s="2"/>
+      <c r="T53" s="2"/>
+      <c r="U53" s="2"/>
+      <c r="V53" s="2"/>
+      <c r="W53" s="2"/>
+      <c r="X53" s="2"/>
+      <c r="Y53" s="2"/>
+      <c r="Z53" s="2"/>
+      <c r="AA53" s="2"/>
+    </row>
+    <row r="54" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" s="17"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="17"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="2"/>
+      <c r="S54" s="2"/>
+      <c r="T54" s="2"/>
+      <c r="U54" s="2"/>
+      <c r="V54" s="2"/>
+      <c r="W54" s="2"/>
+      <c r="X54" s="2"/>
+      <c r="Y54" s="2"/>
+      <c r="Z54" s="2"/>
+      <c r="AA54" s="2"/>
+    </row>
+    <row r="55" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" s="17"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="2"/>
+      <c r="S55" s="2"/>
+      <c r="T55" s="2"/>
+      <c r="U55" s="2"/>
+      <c r="V55" s="2"/>
+      <c r="W55" s="2"/>
+      <c r="X55" s="2"/>
+      <c r="Y55" s="2"/>
+      <c r="Z55" s="2"/>
+      <c r="AA55" s="2"/>
+    </row>
+    <row r="56" spans="1:27" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="19"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="39"/>
+      <c r="J56" s="38"/>
+      <c r="K56" s="39"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="2"/>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
+      <c r="U56" s="2"/>
+      <c r="V56" s="2"/>
+      <c r="W56" s="2"/>
+      <c r="X56" s="2"/>
+      <c r="Y56" s="2"/>
+      <c r="Z56" s="2"/>
+      <c r="AA56" s="2"/>
+    </row>
+    <row r="57" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="20"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2"/>
+      <c r="S57" s="2"/>
+      <c r="T57" s="2"/>
+      <c r="U57" s="2"/>
+      <c r="V57" s="2"/>
+      <c r="W57" s="2"/>
+      <c r="X57" s="2"/>
+      <c r="Y57" s="2"/>
+      <c r="Z57" s="2"/>
+      <c r="AA57" s="2"/>
+    </row>
+    <row r="58" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="23"/>
+      <c r="J58" s="23"/>
+      <c r="K58" s="23"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
+      <c r="R58" s="2"/>
+      <c r="S58" s="2"/>
+      <c r="T58" s="2"/>
+      <c r="U58" s="2"/>
+      <c r="V58" s="2"/>
+      <c r="W58" s="2"/>
+      <c r="X58" s="2"/>
+      <c r="Y58" s="2"/>
+      <c r="Z58" s="2"/>
+      <c r="AA58" s="2"/>
+    </row>
+    <row r="59" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="23"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="23"/>
+      <c r="I59" s="23"/>
+      <c r="J59" s="23"/>
+      <c r="K59" s="23"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="2"/>
+      <c r="Q59" s="2"/>
+      <c r="R59" s="2"/>
+      <c r="S59" s="2"/>
+      <c r="T59" s="2"/>
+      <c r="U59" s="2"/>
+      <c r="V59" s="2"/>
+      <c r="W59" s="2"/>
+      <c r="X59" s="2"/>
+      <c r="Y59" s="2"/>
+      <c r="Z59" s="2"/>
+      <c r="AA59" s="2"/>
+    </row>
+    <row r="60" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="9"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+    </row>
+    <row r="61" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="8"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+    </row>
+    <row r="62" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="8"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+    </row>
+    <row r="63" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B63" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-    </row>
-    <row r="44" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="F44" s="34" t="s">
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+    </row>
+    <row r="64" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="F64" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="G44" s="34"/>
-      <c r="I44" s="34" t="s">
+      <c r="G64" s="43"/>
+      <c r="I64" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="J44" s="34"/>
-    </row>
-    <row r="45" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-    </row>
-    <row r="46" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+      <c r="J64" s="43"/>
+    </row>
+    <row r="65" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="8"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+    </row>
+    <row r="66" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-    </row>
-    <row r="47" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
+    </row>
+    <row r="67" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="11"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="A2:K2"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="I64:J64"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="F10:G10"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="1.0032608695652174" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="78" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Negrita"&amp;8&amp;U
-RECOPILACIÓN DE NORMAS PARA BANCOS Y ENTIDADES FINANCIERAS&amp;R&amp;"Times New Roman,Negrita Cursiva"&amp;7AUTORIDAD DE SUPERVISIÓN DEL SISTEMA FINANCIERO</oddHeader>
-    <oddFooter>&amp;R&amp;"Times New Roman,Normal"&amp;8Libro 5°
+RECOPILACIÓN DE NORMAS PARA SERVICIOS FINANCIEROS&amp;R&amp;"Times New Roman,Negrita Cursiva"&amp;7AUTORIDAD DE SUPERVISIÓN DEL SISTEMA FINANCIERO</oddHeader>
+    <oddFooter>&amp;L&amp;"Times New Roman,Normal"&amp;8Circular ASFI/610/2019 (última)&amp;R&amp;"Times New Roman,Normal"&amp;8Libro 5°
 Título II
 Capítulo III
 Anexo 4.9
-Página &amp;P/1</oddFooter>
+Página &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>